<commit_message>
Corrected CPM and GanttChart. Updated Issues Log and Project Status. Linked style.css file to index.php.
</commit_message>
<xml_diff>
--- a/docs/CPM.xlsx
+++ b/docs/CPM.xlsx
@@ -152,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -265,23 +265,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -316,6 +336,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -600,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,22 +648,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="3"/>
@@ -648,22 +680,22 @@
       <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="13">
         <v>0</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="10">
         <v>0</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="13">
         <v>7</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="10">
         <v>7</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="3"/>
@@ -680,22 +712,22 @@
       <c r="R2" s="3"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="13">
         <v>0</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="10">
         <v>0</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="13">
         <v>7</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="10">
         <v>7</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="3"/>
@@ -712,22 +744,22 @@
       <c r="R3" s="3"/>
     </row>
     <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="13">
         <v>7</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="10">
         <v>7</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="13">
         <v>2</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="10">
         <v>9</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="10">
         <v>0</v>
       </c>
       <c r="G4" s="3"/>
@@ -744,22 +776,22 @@
       <c r="R4" s="3"/>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="13">
         <v>7</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="10">
         <v>7</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="13">
         <v>2</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="10">
         <v>9</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="3"/>
@@ -776,26 +808,26 @@
       <c r="R5" s="3"/>
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="13">
         <v>7</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="10">
         <v>7</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="13">
         <v>2</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="10">
         <v>9</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="10">
         <v>0</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="17"/>
+      <c r="H6" s="15"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -808,22 +840,22 @@
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="13">
         <v>7</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="10">
         <v>7</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="13">
         <v>5</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="10">
         <v>12</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="10">
         <v>0</v>
       </c>
       <c r="G7" s="3"/>
@@ -840,22 +872,22 @@
       <c r="R7" s="3"/>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="13">
         <v>12</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="10">
         <v>12</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="13">
         <v>5</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <v>17</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="10">
         <v>0</v>
       </c>
       <c r="H8" s="3"/>
@@ -903,12 +935,12 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
@@ -926,12 +958,12 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
@@ -949,131 +981,112 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="10"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="8"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
     </row>
     <row r="13" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="5"/>
+      <c r="D13" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="19"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="5"/>
+      <c r="G13" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="19"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="4" t="s">
+      <c r="J13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="N13" s="5"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="10"/>
+      <c r="K13" s="17"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="8"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
     </row>
     <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>16</v>
+      <c r="D14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="7" t="s">
-        <v>17</v>
+      <c r="H14" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="N14" s="7" t="s">
+      <c r="K14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="10"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="8"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
     </row>
     <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>22</v>
+      <c r="E15" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="9" t="s">
-        <v>23</v>
+      <c r="H15" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="I15" s="3"/>
-      <c r="J15" s="8" t="s">
+      <c r="J15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L15" s="3"/>
-      <c r="M15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N15" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="10"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="8"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
@@ -1088,94 +1101,92 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="10"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="8"/>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
     </row>
     <row r="17" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="A17" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="17"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="D17" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="19"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="5"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="10"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="8"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+      <c r="A18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="D18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="10"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="8"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
+      <c r="A19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="D19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
@@ -1190,15 +1201,12 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
@@ -1207,19 +1215,16 @@
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="D21" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="19"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="5"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
@@ -1229,21 +1234,18 @@
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="D22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
@@ -1253,21 +1255,18 @@
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="D23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
@@ -1317,12 +1316,12 @@
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="J13:K13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D21:E21"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A17:B17"/>
     <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="M13:N13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>